<commit_message>
successfully load the data
</commit_message>
<xml_diff>
--- a/backend/db/DANIEL.xlsx
+++ b/backend/db/DANIEL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26200" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3116,7 +3116,7 @@
   <dimension ref="A1:F870"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>